<commit_message>
correction bug et ajout block
</commit_message>
<xml_diff>
--- a/Quete/Aventure.xlsx
+++ b/Quete/Aventure.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\Python_Apprendre_Autrement\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\Python_Apprendre_Autrement\Quete\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D571B6F6-ED90-4F0C-A544-253EB4127EA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F9CBBDC-A678-4AF8-972F-9648C07FDDF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0CA7E0B7-CDFC-4FD5-BEF9-F0FFA02D3C1D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="96">
   <si>
     <t>Chap</t>
   </si>
@@ -72,9 +72,6 @@
   </si>
   <si>
     <t>ID quete</t>
-  </si>
-  <si>
-    <t>Bonjour ?</t>
   </si>
   <si>
     <t xml:space="preserve">Vous voici sur une page où vous allez devoir coder </t>
@@ -421,6 +418,54 @@
 Après chaque maison, tu devras lui dire quel quantité d'eau ammener
 Une fois les 5 maisons éteintes, tu devras annoncer quel quantité d'eau vous avez utilisés
 Une maison avec un incendie de puissance 1, de longueur 1, de largeur 1 et de 1 étage demandera 100mL d'eau </t>
+  </si>
+  <si>
+    <t>Pierre Papier Ciseau</t>
+  </si>
+  <si>
+    <t>Etat de l'eau</t>
+  </si>
+  <si>
+    <t>Liquide</t>
+  </si>
+  <si>
+    <t>Solide</t>
+  </si>
+  <si>
+    <t>Gazeux</t>
+  </si>
+  <si>
+    <t>Écrire un script qui pour une température T donnée affiche l’état de l’eau à cette température c’est-à-dire "Solide", "Liquide" ou "Gazaux". On prendra comme conditions les conditions suivantes : – si la température est strictement négative alors l’eau est à l’état solide ; – si la température est entre 0 et 100 (compris) l’eau est à l’état liquide ; – si la température est strictement supérieure à 100.</t>
+  </si>
+  <si>
+    <t>Moyenne</t>
+  </si>
+  <si>
+    <t>Pour calculer les moyennes de ses étudiants, un professeur calcule la moyenne arithmétique des notes obtenues (le nombre de notes étant fixé à trois) ainsi que la moyenne entre la note la plus basse et la note la plus élevée parmi les 3 notes obtenues. Il choisira par la suite la meilleure des deux moyennes calculées. Ecrire un programme qui saisit les trois notes d’un étudiant et affiche la moyenne finale retenue. Exemple : Si les trois notes d’un étudiant sont : 8.5, 13.5 et 16 alors : — la moyenne arithmétique = (8.5 + 13.5 +16) /3 = 12.667 — la moyenne de la note la plus basse et la plus élevée = (8.5+16) /2 = 12.25 Le professeur choisira la moyenne arithmétique.</t>
+  </si>
+  <si>
+    <t>10
+15
+8</t>
+  </si>
+  <si>
+    <t>La moyenne retenue est la moyenne des trois notes :  11.0</t>
+  </si>
+  <si>
+    <t>11
+12
+18</t>
+  </si>
+  <si>
+    <t>La moyenne retenue est celle des 2 notes :  14.5</t>
+  </si>
+  <si>
+    <t>12
+1
+10</t>
+  </si>
+  <si>
+    <t>La moyenne retenue est la moyenne des trois notes :  7.666666666666667</t>
   </si>
 </sst>
 </file>
@@ -804,10 +849,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95F0EE0D-D391-4AA7-AF3E-FA9E64764AC4}">
-  <dimension ref="A1:Y9"/>
+  <dimension ref="A1:Y11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F4" zoomScale="97" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+    <sheetView tabSelected="1" zoomScale="97" workbookViewId="0">
+      <selection activeCell="T14" sqref="T14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -838,13 +883,13 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>3</v>
@@ -868,34 +913,34 @@
         <v>9</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="R1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="X1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y1" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:25" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -903,7 +948,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" s="1">
         <v>0</v>
@@ -912,31 +957,31 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="P2" s="1"/>
       <c r="Q2" s="1">
@@ -944,7 +989,7 @@
       </c>
       <c r="R2" s="1"/>
       <c r="S2" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
@@ -958,7 +1003,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
@@ -967,16 +1012,16 @@
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="H3" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I3" s="1">
         <v>6</v>
@@ -988,41 +1033,41 @@
         <v>14</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="N3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="P3" s="1"/>
       <c r="Q3" s="1">
         <v>4</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="S3" s="1">
         <v>6</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="U3" s="1">
         <v>7</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="W3" s="1">
         <v>14</v>
       </c>
       <c r="X3" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="Y3" s="2">
         <v>11</v>
@@ -1033,7 +1078,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C4" s="1">
         <v>2</v>
@@ -1043,56 +1088,56 @@
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="H4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="L4" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="M4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="O4" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>80</v>
       </c>
       <c r="P4" s="1"/>
       <c r="Q4" s="1">
         <v>3</v>
       </c>
       <c r="R4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="S4" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="S4" s="1" t="s">
+      <c r="T4" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="T4" s="1" t="s">
+      <c r="U4" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="V4" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="U4" s="1" t="s">
+      <c r="W4" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="V4" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="W4" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
@@ -1102,7 +1147,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C5" s="1">
         <v>3</v>
@@ -1130,7 +1175,7 @@
         <v>16</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
@@ -1169,7 +1214,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C6" s="1">
         <v>4</v>
@@ -1188,16 +1233,16 @@
         <v>5</v>
       </c>
       <c r="I6" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="K6" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="L6" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
@@ -1210,25 +1255,25 @@
         <v>2</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="T6" s="1">
         <v>3</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="V6" s="1">
         <v>5</v>
       </c>
       <c r="W6" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="X6" s="1">
         <v>25</v>
       </c>
       <c r="Y6" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="129.6" x14ac:dyDescent="0.3">
@@ -1236,7 +1281,7 @@
         <v>0</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C7" s="1">
         <v>5</v>
@@ -1264,7 +1309,7 @@
         <v>64</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
@@ -1303,7 +1348,7 @@
         <v>0</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C8" s="1">
         <v>6</v>
@@ -1312,16 +1357,16 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="I8" s="1">
         <v>97</v>
@@ -1333,7 +1378,7 @@
         <v>67</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
@@ -1343,19 +1388,19 @@
         <v>3</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="S8" s="1">
         <v>97</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="U8" s="1">
         <v>77</v>
       </c>
       <c r="V8" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="W8" s="1">
         <v>46</v>
@@ -1365,10 +1410,10 @@
     </row>
     <row r="9" spans="1:25" ht="331.2" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>12</v>
+        <v>82</v>
       </c>
       <c r="C9" s="1">
         <v>7</v>
@@ -1377,64 +1422,176 @@
         <v>0</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="I9" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="K9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="L9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="L9" s="1" t="s">
+      <c r="M9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="M9" s="1" t="s">
+      <c r="N9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="N9" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="O9" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q9" s="1">
         <v>3</v>
       </c>
       <c r="R9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="T9" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="S9" s="1" t="s">
+      <c r="U9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="T9" s="1" t="s">
+      <c r="V9" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="U9" s="1" t="s">
+      <c r="W9" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="V9" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="W9" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="X9" s="1"/>
       <c r="Y9" s="1"/>
+    </row>
+    <row r="10" spans="1:25" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>1</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" s="1">
+        <v>8</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1">
+        <v>10</v>
+      </c>
+      <c r="G10" s="1">
+        <v>-12</v>
+      </c>
+      <c r="H10" s="1">
+        <v>126</v>
+      </c>
+      <c r="I10" t="s">
+        <v>84</v>
+      </c>
+      <c r="J10" t="s">
+        <v>85</v>
+      </c>
+      <c r="K10" t="s">
+        <v>86</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>3</v>
+      </c>
+      <c r="R10" s="1">
+        <v>10</v>
+      </c>
+      <c r="S10" t="s">
+        <v>84</v>
+      </c>
+      <c r="T10" s="1">
+        <v>-10</v>
+      </c>
+      <c r="U10" t="s">
+        <v>85</v>
+      </c>
+      <c r="V10" s="1">
+        <v>127</v>
+      </c>
+      <c r="W10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C11" s="1">
+        <v>9</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>3</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="T11" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="U11" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="V11" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="W11" s="1" t="s">
+        <v>95</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Lecture direct excel + finition taverne minotaur
</commit_message>
<xml_diff>
--- a/Quete/Aventure.xlsx
+++ b/Quete/Aventure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\Python_Apprendre_Autrement\Quete\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F9CBBDC-A678-4AF8-972F-9648C07FDDF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65439E1F-FDE2-49E7-9EDE-579756F6F738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0CA7E0B7-CDFC-4FD5-BEF9-F0FFA02D3C1D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="52">
   <si>
     <t>Chap</t>
   </si>
@@ -74,27 +74,6 @@
     <t>ID quete</t>
   </si>
   <si>
-    <t xml:space="preserve">Vous voici sur une page où vous allez devoir coder </t>
-  </si>
-  <si>
-    <t>J2 gagne</t>
-  </si>
-  <si>
-    <t>J1 gagne</t>
-  </si>
-  <si>
-    <t>Egalité</t>
-  </si>
-  <si>
-    <t>Un groupe d'enfant vous a demandé de créer un pierre papier ciseaux, vous devrez donc, dans votre progamme, demander a chacun des participant, si il veut jouer "Pierre", "Papier","Ciseaux" et d'afficher le resultat "J2 gagne", "J1 gagne" Egalité</t>
-  </si>
-  <si>
-    <t>N'ayez pas peur de preparer tous les cas possibles</t>
-  </si>
-  <si>
-    <t>il y a le cas J1 joue "Pierre" et J2 joue "Ciseaux", si vous voyez cela, le joueur 1 gagne</t>
-  </si>
-  <si>
     <t>input_test_1</t>
   </si>
   <si>
@@ -116,9 +95,6 @@
     <t>Code_init</t>
   </si>
   <si>
-    <t>print("Hello World")</t>
-  </si>
-  <si>
     <t>input_exemple_1</t>
   </si>
   <si>
@@ -126,18 +102,6 @@
   </si>
   <si>
     <t>input_exemple_2</t>
-  </si>
-  <si>
-    <t>voici le début d'un code fonctionnel : 
-J1 =input("Pierre, Papier ou Ciseaux: ")
-J2 = input("Pierre, Papier ou Ciseaux: ")
-if J1 == J2:
-    print('Egalité')
-elif J1 == "Pierre" and J2 == "Papier":
-    print("J2 gagne")
-    pass
-elif J1 == "Pierre" and J2 == "Ciseaux":
-    print("J1 gagne")</t>
   </si>
   <si>
     <t>Je vais bien</t>
@@ -183,18 +147,6 @@
     <t>4
 2
 1</t>
-  </si>
-  <si>
-    <t>Pierre
-Papier</t>
-  </si>
-  <si>
-    <t>Papier
-Pierre</t>
-  </si>
-  <si>
-    <t>Papier
-Papier</t>
   </si>
   <si>
     <t>input_test_4</t>
@@ -229,68 +181,6 @@
 ici, la variable nombre aura alors la valeur entrée par l'utilisateur
 Si jamais on a besoin de stoquer une deuxieme valeur, on utilisera alors une autre variable
 nombre2 = int(input())</t>
-  </si>
-  <si>
-    <t>Ecrivez une fonction qui prend un entier positif ‘num’ et calcule combien de points existent dans une forme pentagonale autour du point central à la Nième itération. Dans l'image ci-dessous, vous pouvez voir que la première itération ne comporte qu'un seul point. À la deuxième itération, il y a 6 points. Sur la troisième, il y a 16 points, et sur la quatrième, il y a 31 points. Renvoie le nombre de points qui existent dans le pentagone entier à la Nième itération.</t>
-  </si>
-  <si>
-    <t>Pentagone</t>
-  </si>
-  <si>
-    <t>Ecrire un programme qui demande à l'utilisateur de saisir un nombre entier N et d’afficher la valeur et le type de son carré, sa division par 3 et sa division entière par 5 ;</t>
-  </si>
-  <si>
-    <t>Operation</t>
-  </si>
-  <si>
-    <t>Cube</t>
-  </si>
-  <si>
-    <t>Ecrire un programme qui demande à l'utilisateur de saisir : un nombre réel F et d’afficher son cube</t>
-  </si>
-  <si>
-    <t>Ascii code</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>Pour un char un caractère Ch et d’afficher son code ascii</t>
-  </si>
-  <si>
-    <t>@</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>.</t>
-  </si>
-  <si>
-    <t>Pour obtenir le code ascii d'un char, utilise la fonction ord()</t>
-  </si>
-  <si>
-    <t>4
-0.6666666666666666
-0</t>
-  </si>
-  <si>
-    <t>9
-1.0
-0</t>
-  </si>
-  <si>
-    <t>25
-1.6666666666666667
-1</t>
-  </si>
-  <si>
-    <t>625
-8.333333333333334
-5</t>
   </si>
   <si>
     <t>Compte les champignons pour savoir combien vous en avez
@@ -418,54 +308,6 @@
 Après chaque maison, tu devras lui dire quel quantité d'eau ammener
 Une fois les 5 maisons éteintes, tu devras annoncer quel quantité d'eau vous avez utilisés
 Une maison avec un incendie de puissance 1, de longueur 1, de largeur 1 et de 1 étage demandera 100mL d'eau </t>
-  </si>
-  <si>
-    <t>Pierre Papier Ciseau</t>
-  </si>
-  <si>
-    <t>Etat de l'eau</t>
-  </si>
-  <si>
-    <t>Liquide</t>
-  </si>
-  <si>
-    <t>Solide</t>
-  </si>
-  <si>
-    <t>Gazeux</t>
-  </si>
-  <si>
-    <t>Écrire un script qui pour une température T donnée affiche l’état de l’eau à cette température c’est-à-dire "Solide", "Liquide" ou "Gazaux". On prendra comme conditions les conditions suivantes : – si la température est strictement négative alors l’eau est à l’état solide ; – si la température est entre 0 et 100 (compris) l’eau est à l’état liquide ; – si la température est strictement supérieure à 100.</t>
-  </si>
-  <si>
-    <t>Moyenne</t>
-  </si>
-  <si>
-    <t>Pour calculer les moyennes de ses étudiants, un professeur calcule la moyenne arithmétique des notes obtenues (le nombre de notes étant fixé à trois) ainsi que la moyenne entre la note la plus basse et la note la plus élevée parmi les 3 notes obtenues. Il choisira par la suite la meilleure des deux moyennes calculées. Ecrire un programme qui saisit les trois notes d’un étudiant et affiche la moyenne finale retenue. Exemple : Si les trois notes d’un étudiant sont : 8.5, 13.5 et 16 alors : — la moyenne arithmétique = (8.5 + 13.5 +16) /3 = 12.667 — la moyenne de la note la plus basse et la plus élevée = (8.5+16) /2 = 12.25 Le professeur choisira la moyenne arithmétique.</t>
-  </si>
-  <si>
-    <t>10
-15
-8</t>
-  </si>
-  <si>
-    <t>La moyenne retenue est la moyenne des trois notes :  11.0</t>
-  </si>
-  <si>
-    <t>11
-12
-18</t>
-  </si>
-  <si>
-    <t>La moyenne retenue est celle des 2 notes :  14.5</t>
-  </si>
-  <si>
-    <t>12
-1
-10</t>
-  </si>
-  <si>
-    <t>La moyenne retenue est la moyenne des trois notes :  7.666666666666667</t>
   </si>
 </sst>
 </file>
@@ -851,8 +693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95F0EE0D-D391-4AA7-AF3E-FA9E64764AC4}">
   <dimension ref="A1:Y11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="97" workbookViewId="0">
-      <selection activeCell="T14" sqref="T14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="71" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -883,13 +725,13 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>3</v>
@@ -913,34 +755,34 @@
         <v>9</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:25" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -948,7 +790,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="C2" s="1">
         <v>0</v>
@@ -957,31 +799,31 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P2" s="1"/>
       <c r="Q2" s="1">
@@ -989,7 +831,7 @@
       </c>
       <c r="R2" s="1"/>
       <c r="S2" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
@@ -1003,7 +845,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
@@ -1012,16 +854,16 @@
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="I3" s="1">
         <v>6</v>
@@ -1033,41 +875,41 @@
         <v>14</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="P3" s="1"/>
       <c r="Q3" s="1">
         <v>4</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="S3" s="1">
         <v>6</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="U3" s="1">
         <v>7</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="W3" s="1">
         <v>14</v>
       </c>
       <c r="X3" s="1" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="Y3" s="2">
         <v>11</v>
@@ -1078,7 +920,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="C4" s="1">
         <v>2</v>
@@ -1088,510 +930,228 @@
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>71</v>
+        <v>41</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>74</v>
+        <v>44</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>72</v>
+        <v>42</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>75</v>
+        <v>45</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>76</v>
+        <v>46</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>81</v>
+        <v>51</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>77</v>
+        <v>47</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>78</v>
+        <v>48</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="P4" s="1"/>
       <c r="Q4" s="1">
         <v>3</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>71</v>
+        <v>41</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>72</v>
+        <v>42</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>75</v>
+        <v>45</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>74</v>
+        <v>44</v>
       </c>
       <c r="W4" s="1" t="s">
-        <v>76</v>
+        <v>46</v>
       </c>
       <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
     </row>
-    <row r="5" spans="1:25" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C5" s="1">
-        <v>3</v>
-      </c>
-      <c r="D5" s="1">
-        <v>2</v>
-      </c>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="1">
-        <v>1</v>
-      </c>
-      <c r="G5" s="1">
-        <v>2</v>
-      </c>
-      <c r="H5" s="1">
-        <v>3</v>
-      </c>
-      <c r="I5" s="1">
-        <v>1</v>
-      </c>
-      <c r="J5" s="1">
-        <v>5</v>
-      </c>
-      <c r="K5" s="1">
-        <v>16</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>52</v>
-      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
-      <c r="Q5" s="1">
-        <v>4</v>
-      </c>
-      <c r="R5" s="1">
-        <v>1</v>
-      </c>
-      <c r="S5" s="1">
-        <v>1</v>
-      </c>
-      <c r="T5" s="1">
-        <v>8</v>
-      </c>
-      <c r="U5" s="1">
-        <v>141</v>
-      </c>
-      <c r="V5" s="1">
-        <v>10</v>
-      </c>
-      <c r="W5" s="1">
-        <v>226</v>
-      </c>
-      <c r="X5" s="1">
-        <v>15</v>
-      </c>
-      <c r="Y5" s="1">
-        <v>526</v>
-      </c>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
+      <c r="Y5" s="1"/>
     </row>
-    <row r="6" spans="1:25" ht="216" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>0</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C6" s="1">
-        <v>4</v>
-      </c>
-      <c r="D6" s="1">
-        <v>1</v>
-      </c>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="1">
-        <v>2</v>
-      </c>
-      <c r="G6" s="1">
-        <v>3</v>
-      </c>
-      <c r="H6" s="1">
-        <v>5</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>54</v>
-      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
-      <c r="Q6" s="1">
-        <v>4</v>
-      </c>
-      <c r="R6" s="1">
-        <v>2</v>
-      </c>
-      <c r="S6" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="T6" s="1">
-        <v>3</v>
-      </c>
-      <c r="U6" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="V6" s="1">
-        <v>5</v>
-      </c>
-      <c r="W6" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="X6" s="1">
-        <v>25</v>
-      </c>
-      <c r="Y6" s="1" t="s">
-        <v>69</v>
-      </c>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="W6" s="1"/>
+      <c r="X6" s="1"/>
+      <c r="Y6" s="1"/>
     </row>
-    <row r="7" spans="1:25" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <v>0</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C7" s="1">
-        <v>5</v>
-      </c>
-      <c r="D7" s="1">
-        <v>1</v>
-      </c>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="1">
-        <v>2</v>
-      </c>
-      <c r="G7" s="1">
-        <v>3</v>
-      </c>
-      <c r="H7" s="1">
-        <v>4</v>
-      </c>
-      <c r="I7" s="1">
-        <v>8</v>
-      </c>
-      <c r="J7" s="1">
-        <v>27</v>
-      </c>
-      <c r="K7" s="1">
-        <v>64</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>57</v>
-      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
-      <c r="Q7" s="1">
-        <v>4</v>
-      </c>
-      <c r="R7" s="1">
-        <v>2</v>
-      </c>
-      <c r="S7" s="1">
-        <v>8</v>
-      </c>
-      <c r="T7" s="1">
-        <v>3</v>
-      </c>
-      <c r="U7" s="1">
-        <v>27</v>
-      </c>
-      <c r="V7" s="1">
-        <v>4</v>
-      </c>
-      <c r="W7" s="1">
-        <v>64</v>
-      </c>
-      <c r="X7" s="1">
-        <v>10</v>
-      </c>
-      <c r="Y7" s="1">
-        <v>1000</v>
-      </c>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
+      <c r="X7" s="1"/>
+      <c r="Y7" s="1"/>
     </row>
-    <row r="8" spans="1:25" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
-        <v>0</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C8" s="1">
-        <v>6</v>
-      </c>
-      <c r="D8" s="1">
-        <v>1</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="I8" s="1">
-        <v>97</v>
-      </c>
-      <c r="J8" s="1">
-        <v>64</v>
-      </c>
-      <c r="K8" s="1">
-        <v>67</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>60</v>
-      </c>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
-      <c r="Q8" s="1">
-        <v>3</v>
-      </c>
-      <c r="R8" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="S8" s="1">
-        <v>97</v>
-      </c>
-      <c r="T8" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="U8" s="1">
-        <v>77</v>
-      </c>
-      <c r="V8" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="W8" s="1">
-        <v>46</v>
-      </c>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="1"/>
       <c r="X8" s="1"/>
       <c r="Y8" s="1"/>
     </row>
-    <row r="9" spans="1:25" ht="331.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
-        <v>1</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C9" s="1">
-        <v>7</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q9" s="1">
-        <v>3</v>
-      </c>
-      <c r="R9" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="S9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="T9" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="U9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="V9" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="W9" s="1" t="s">
-        <v>15</v>
-      </c>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="1"/>
+      <c r="V9" s="1"/>
+      <c r="W9" s="1"/>
       <c r="X9" s="1"/>
       <c r="Y9" s="1"/>
     </row>
-    <row r="10" spans="1:25" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
-        <v>1</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C10" s="1">
-        <v>8</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0</v>
-      </c>
-      <c r="F10" s="1">
-        <v>10</v>
-      </c>
-      <c r="G10" s="1">
-        <v>-12</v>
-      </c>
-      <c r="H10" s="1">
-        <v>126</v>
-      </c>
-      <c r="I10" t="s">
-        <v>84</v>
-      </c>
-      <c r="J10" t="s">
-        <v>85</v>
-      </c>
-      <c r="K10" t="s">
-        <v>86</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q10" s="1">
-        <v>3</v>
-      </c>
-      <c r="R10" s="1">
-        <v>10</v>
-      </c>
-      <c r="S10" t="s">
-        <v>84</v>
-      </c>
-      <c r="T10" s="1">
-        <v>-10</v>
-      </c>
-      <c r="U10" t="s">
-        <v>85</v>
-      </c>
-      <c r="V10" s="1">
-        <v>127</v>
-      </c>
-      <c r="W10" t="s">
-        <v>86</v>
-      </c>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="V10" s="1"/>
     </row>
-    <row r="11" spans="1:25" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
-        <v>1</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C11" s="1">
-        <v>9</v>
-      </c>
-      <c r="D11" s="1">
-        <v>1</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="Q11" s="1">
-        <v>3</v>
-      </c>
-      <c r="R11" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="S11" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="T11" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="U11" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="V11" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="W11" s="1" t="s">
-        <v>95</v>
-      </c>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+      <c r="W11" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
ajout systeme de point variant selon le chap
</commit_message>
<xml_diff>
--- a/Quete/Aventure.xlsx
+++ b/Quete/Aventure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\Python_Apprendre_Autrement\Quete\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF0BE812-CCB3-486C-B9CD-836EE7BB1B67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D51B72-8D7F-4FCC-BADF-341F65730191}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0CA7E0B7-CDFC-4FD5-BEF9-F0FFA02D3C1D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="64">
   <si>
     <t>Chap</t>
   </si>
@@ -734,8 +734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95F0EE0D-D391-4AA7-AF3E-FA9E64764AC4}">
   <dimension ref="A1:Y11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="71" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" topLeftCell="D4" zoomScale="71" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1025,33 +1025,66 @@
       <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>2</v>
       </c>
-      <c r="B5" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="C5" s="1">
         <v>3</v>
       </c>
-      <c r="D5" s="1"/>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
       <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
+      <c r="F5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="1"/>
-      <c r="S5" s="1"/>
-      <c r="T5" s="1"/>
-      <c r="U5" s="1"/>
-      <c r="V5" s="1"/>
-      <c r="W5" s="1"/>
+      <c r="Q5" s="1">
+        <v>3</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="X5" s="1"/>
       <c r="Y5" s="1"/>
     </row>

</xml_diff>

<commit_message>
correction img + quete
</commit_message>
<xml_diff>
--- a/Quete/Aventure.xlsx
+++ b/Quete/Aventure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\Python_Apprendre_Autrement\Quete\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A6548B9-92C9-4121-844C-C24BBBE4767E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C7ACBEE-7E44-40A5-88C3-CD07D83A90D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0CA7E0B7-CDFC-4FD5-BEF9-F0FFA02D3C1D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="68">
   <si>
     <t>Chap</t>
   </si>
@@ -355,6 +355,12 @@
   </si>
   <si>
     <t>Forge la lane</t>
+  </si>
+  <si>
+    <t>0.1</t>
+  </si>
+  <si>
+    <t>0.2</t>
   </si>
 </sst>
 </file>
@@ -740,8 +746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95F0EE0D-D391-4AA7-AF3E-FA9E64764AC4}">
   <dimension ref="A1:Y11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="71" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="71" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -842,8 +848,8 @@
       <c r="C2" s="1">
         <v>0</v>
       </c>
-      <c r="D2" s="1">
-        <v>0</v>
+      <c r="D2" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>38</v>
@@ -897,8 +903,8 @@
       <c r="C3" s="1">
         <v>1</v>
       </c>
-      <c r="D3" s="1">
-        <v>0</v>
+      <c r="D3" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>39</v>
@@ -973,7 +979,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">

</xml_diff>

<commit_message>
Forgeron + quete correction
</commit_message>
<xml_diff>
--- a/Quete/Aventure.xlsx
+++ b/Quete/Aventure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\Python_Apprendre_Autrement\Quete\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A330A6D-9556-48DD-8F6D-23E9C56ED0B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55C9035A-991D-4A7A-AC62-90C34E60FAEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0CA7E0B7-CDFC-4FD5-BEF9-F0FFA02D3C1D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="89">
   <si>
     <t>Chap</t>
   </si>
@@ -187,96 +187,6 @@
 Il y a ici 3 types de champignons</t>
   </si>
   <si>
-    <t>1
-5
-4
-2
-2
-3
-2
-1
-6
-4
-5
-2
-5
-2
-3
-1
-4
-6
-3
-1</t>
-  </si>
-  <si>
-    <t>Il faut apporter 4000mL d'eau pour la maison 1
-Il faut apporter 1200mL d'eau pour la maison 2
-Il faut apporter 24000mL d'eau pour la maison 3
-Il faut apporter 3000mL d'eau pour la maison 4
-Il faut apporter 7200mL d'eau pour la maison 5
-Il faut apporter 39400mL d'eau au total</t>
-  </si>
-  <si>
-    <t>2
-4
-6
-2
-1
-3
-2
-1
-5
-4
-5
-2
-6
-2
-3
-1
-4
-6
-2
-1</t>
-  </si>
-  <si>
-    <t>1
-1
-1
-2
-2
-3
-2
-1
-1
-4
-5
-2
-7
-2
-3
-1
-5
-6
-3
-2</t>
-  </si>
-  <si>
-    <t>Il faut apporter 9600mL d'eau pour la maison 1
-Il faut apporter 600mL d'eau pour la maison 2
-Il faut apporter 20000mL d'eau pour la maison 3
-Il faut apporter 3600mL d'eau pour la maison 4
-Il faut apporter 4800mL d'eau pour la maison 5
-Il faut apporter 38600mL d'eau au total</t>
-  </si>
-  <si>
-    <t>Il faut apporter 200mL d'eau pour la maison 1
-Il faut apporter 1200mL d'eau pour la maison 2
-Il faut apporter 4000mL d'eau pour la maison 3
-Il faut apporter 4200mL d'eau pour la maison 4
-Il faut apporter 18000mL d'eau pour la maison 5
-Il faut apporter 27600mL d'eau au total</t>
-  </si>
-  <si>
     <t>Multiplie chacune des valeurs pour obtenir le volume de flamme à éteindre</t>
   </si>
   <si>
@@ -296,20 +206,6 @@
     <t>Arrete l'incendie</t>
   </si>
   <si>
-    <t xml:space="preserve">Vite tu dois arreter l'incendie
-Il y a 5 maisons mais tu ne sais pas a l'avance quelle quantité d'eau tu as besoin
-Navi est partie te dire l'étendue des flammes pendant que tu es parti cherché de l'eau
-Navi te dire les informations dans l'ordre suivant:
-la puissance des flammes
-la longueur de la maison
-la largeur de la maison
-la nombre d'étage de la maison
-Elle répetera ces informations pour les 5 maisons
-Après chaque maison, tu devras lui dire quel quantité d'eau ammener
-Une fois les 5 maisons éteintes, tu devras annoncer quel quantité d'eau vous avez utilisés
-Une maison avec un incendie de puissance 1, de longueur 1, de largeur 1 et de 1 étage demandera 100mL d'eau </t>
-  </si>
-  <si>
     <t>Dechiffrer le message</t>
   </si>
   <si>
@@ -456,6 +352,137 @@
 -39
 5
 J'ai attrapé 6 pommes</t>
+  </si>
+  <si>
+    <t>Trouve ton chemin</t>
+  </si>
+  <si>
+    <t>Devant toi se trouve trois portes
+En reseolvant cette enigme, vous trouvez la porte à prendre
+Pour un entier n donné
+Determiner si celui çi est pair,s'il est divisible par 3 et ou s'il est divisible par 7 ou aucun des 3
+Exemple : Pour un entier 42,
+La réponse sera : 
+42 est divisible par
+2
+3
+7</t>
+  </si>
+  <si>
+    <t>60 est divisible par
+2
+3</t>
+  </si>
+  <si>
+    <t>41 n'est divisible par aucun des trois nombres</t>
+  </si>
+  <si>
+    <t>84 est divisible par
+2
+3
+7</t>
+  </si>
+  <si>
+    <t>43 n'est divisible par aucun des trois nombres</t>
+  </si>
+  <si>
+    <t>40 est divisible par
+2</t>
+  </si>
+  <si>
+    <t>168 est divisible par
+2
+3
+7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vite tu dois arreter l'incendie
+Tu vas recevoir les dimensions de 2 maisons par 2 maisons
+Navi est partie te dire l'étendue des flammes pendant que tu es parti cherché de l'eau
+Navi va te dire les informations dans l'ordre suivant:
+la puissance des flammes
+la longueur de la maison
+la largeur de la maison
+la nombre d'étage de la maison
+Elle répetera ces informations pour les 2 maisons
+Après chaque maison, tu devras lui dire quel quantité d'eau ammener
+Une fois les 2 maisons éteintes, tu devras annoncer quel quantité d'eau vous avez utilisés
+Une maison avec un incendie de puissance 1, de longueur 1, de largeur 1 et de 1 étage demandera 100mL d'eau </t>
+  </si>
+  <si>
+    <t>1
+5
+4
+2
+2
+3
+2
+1</t>
+  </si>
+  <si>
+    <t>2
+4
+6
+2
+1
+3
+2
+1</t>
+  </si>
+  <si>
+    <t>1
+1
+1
+2
+2
+3
+2
+1</t>
+  </si>
+  <si>
+    <t>Il faut apporter 4000mL d'eau pour la maison 1
+Il faut apporter 1200mL d'eau pour la maison 2
+Il faut apporter 5200mL d'eau au total</t>
+  </si>
+  <si>
+    <t>Il faut apporter 9600mL d'eau pour la maison 1
+Il faut apporter 600mL d'eau pour la maison 2
+Il faut apporter 10200mL d'eau au total</t>
+  </si>
+  <si>
+    <t>Il faut apporter 200mL d'eau pour la maison 1
+Il faut apporter 1200mL d'eau pour la maison 2
+Il faut apporter 1400mL d'eau au total</t>
+  </si>
+  <si>
+    <t>5
+2
+1
+5
+3
+1
+6
+8</t>
+  </si>
+  <si>
+    <t>Il faut apporter 5000mL d'eau pour la maison 1
+Il faut apporter 14400mL d'eau pour la maison 2
+Il faut apporter 19400mL d'eau au total</t>
+  </si>
+  <si>
+    <t>2
+1
+6
+1
+4
+3
+1
+2</t>
+  </si>
+  <si>
+    <t>Il faut apporter 1200mL d'eau pour la maison 1
+Il faut apporter 2400mL d'eau pour la maison 2
+Il faut apporter 3600mL d'eau au total</t>
   </si>
 </sst>
 </file>
@@ -841,8 +868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95F0EE0D-D391-4AA7-AF3E-FA9E64764AC4}">
   <dimension ref="A1:Y11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="56" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="X8" sqref="X8"/>
+    <sheetView tabSelected="1" topLeftCell="H5" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -944,7 +971,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>38</v>
@@ -999,7 +1026,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>39</v>
@@ -1063,12 +1090,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="409.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C4" s="1">
         <v>2</v>
@@ -1078,66 +1105,66 @@
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="N4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O4" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="P4" s="1"/>
       <c r="Q4" s="1">
         <v>3</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>41</v>
+        <v>79</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>42</v>
+        <v>82</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>43</v>
+        <v>85</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>45</v>
+        <v>86</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>44</v>
+        <v>87</v>
       </c>
       <c r="W4" s="1" t="s">
-        <v>46</v>
+        <v>88</v>
       </c>
       <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
     </row>
-    <row r="5" spans="1:25" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
       <c r="C5" s="1">
         <v>3</v>
@@ -1146,61 +1173,65 @@
         <v>0</v>
       </c>
       <c r="E5" s="1"/>
-      <c r="F5" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>57</v>
+      <c r="F5" s="1">
+        <v>60</v>
+      </c>
+      <c r="G5" s="1">
+        <v>41</v>
+      </c>
+      <c r="H5" s="1">
+        <v>84</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1">
-        <v>3</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>53</v>
+        <v>4</v>
+      </c>
+      <c r="R5" s="1">
+        <v>60</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="T5" s="1" t="s">
-        <v>60</v>
+        <v>72</v>
+      </c>
+      <c r="T5" s="1">
+        <v>43</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="V5" s="1" t="s">
-        <v>62</v>
+        <v>75</v>
+      </c>
+      <c r="V5" s="1">
+        <v>84</v>
       </c>
       <c r="W5" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="X5" s="1"/>
-      <c r="Y5" s="1"/>
+        <v>76</v>
+      </c>
+      <c r="X5" s="1">
+        <v>168</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="6" spans="1:25" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C6" s="1">
         <v>4</v>
@@ -1210,25 +1241,25 @@
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
@@ -1238,22 +1269,22 @@
         <v>3</v>
       </c>
       <c r="R6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="T6" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="S6" s="1" t="s">
+      <c r="U6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="V6" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="T6" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="U6" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="V6" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="W6" s="1" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="X6" s="1"/>
       <c r="Y6" s="1"/>
@@ -1263,7 +1294,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C7" s="1">
         <v>5</v>
@@ -1273,25 +1304,25 @@
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
@@ -1301,22 +1332,22 @@
         <v>3</v>
       </c>
       <c r="R7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="V7" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="S7" s="1" t="s">
+      <c r="W7" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="T7" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="U7" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="V7" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="W7" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="X7" s="1"/>
       <c r="Y7" s="1"/>
@@ -1326,7 +1357,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C8" s="1">
         <v>6</v>
@@ -1336,25 +1367,25 @@
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
@@ -1364,22 +1395,22 @@
         <v>3</v>
       </c>
       <c r="R8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="V8" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="S8" s="1" t="s">
+      <c r="W8" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="T8" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="U8" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="V8" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="W8" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="X8" s="1"/>
       <c r="Y8" s="1"/>

</xml_diff>

<commit_message>
ajout test lecture config
</commit_message>
<xml_diff>
--- a/Quete/Aventure.xlsx
+++ b/Quete/Aventure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\Python_Apprendre_Autrement\Quete\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55C9035A-991D-4A7A-AC62-90C34E60FAEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23C4F6DD-91D1-48BE-8C98-D5E3B2296301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0CA7E0B7-CDFC-4FD5-BEF9-F0FFA02D3C1D}"/>
+    <workbookView xWindow="5760" yWindow="1044" windowWidth="17280" windowHeight="9420" xr2:uid="{0CA7E0B7-CDFC-4FD5-BEF9-F0FFA02D3C1D}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -869,7 +869,7 @@
   <dimension ref="A1:Y11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H5" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Ajout quete forge + correction bug
</commit_message>
<xml_diff>
--- a/Quete/Aventure.xlsx
+++ b/Quete/Aventure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\Python_Apprendre_Autrement\Quete\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23C4F6DD-91D1-48BE-8C98-D5E3B2296301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51BAE790-1932-41AC-BB9B-88717A7FE457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="1044" windowWidth="17280" windowHeight="9420" xr2:uid="{0CA7E0B7-CDFC-4FD5-BEF9-F0FFA02D3C1D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0CA7E0B7-CDFC-4FD5-BEF9-F0FFA02D3C1D}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="98">
   <si>
     <t>Chap</t>
   </si>
@@ -484,12 +484,170 @@
 Il faut apporter 2400mL d'eau pour la maison 2
 Il faut apporter 3600mL d'eau au total</t>
   </si>
+  <si>
+    <t>60.2</t>
+  </si>
+  <si>
+    <t>Attends, la lance est à 100.00 degré
+Attends, la lance est à 92.00 degré
+Coup 1: Frappe a gauche, la lance est à 84.64 degré
+Coup 2: Frappe a droite, la lance est à 77.87 degré
+Coup 3: Frappe a droite, la lance est à 71.64 degré
+Coup 4: Frappe au centre, la lance est à 65.91 degré
+Coup 5: Frappe au centre, la lance est à 60.64 degré
+Coup 6: Frappe au centre, la lance est à 55.78 degré
+Coup 7: Frappe au centre, la lance est à 51.32 degré
+Rechauffe 1: de 47.22 à 97.22 degré
+Attends, la lance est à 97.22 degré
+Coup 8: Frappe a gauche, la lance est à 89.44 degré
+Coup 9: Frappe a gauche, la lance est à 82.28 degré
+Coup 10: Frappe a droite, la lance est à 75.70 degré
+Coup 11: Frappe au centre, la lance est à 69.64 degré
+Coup 12: Frappe au centre, la lance est à 64.07 degré
+Coup 13: Frappe au centre, la lance est à 58.95 degré
+Coup 14: Frappe au centre, la lance est à 54.23 degré
+Rechauffe 2: de 49.89 à 99.89 degré
+Attends, la lance est à 99.89 degré
+Attends, la lance est à 91.90 degré
+Coup 15: Frappe a gauche, la lance est à 84.55 degré
+Coup 16: Frappe a droite, la lance est à 77.79 degré
+Coup 17: Frappe a droite, la lance est à 71.56 degré
+Coup 18: Frappe au centre, la lance est à 65.84 degré
+Coup 19: Frappe au centre, la lance est à 60.57 degré
+Coup 20: Frappe au centre, la lance est à 55.73 degré</t>
+  </si>
+  <si>
+    <t>Rechauffe 1: de 50.00 à 100.00 degré
+Attends, la lance est à 100.00 degré
+Attends, la lance est à 92.00 degré
+Coup 1: Frappe a gauche, la lance est à 84.64 degré
+Coup 2: Frappe a droite, la lance est à 77.87 degré
+Coup 3: Frappe a droite, la lance est à 71.64 degré
+Coup 4: Frappe au centre, la lance est à 65.91 degré
+Coup 5: Frappe au centre, la lance est à 60.64 degré
+Coup 6: Frappe au centre, la lance est à 55.78 degré
+Coup 7: Frappe au centre, la lance est à 51.32 degré
+Rechauffe 2: de 47.22 à 97.22 degré
+Attends, la lance est à 97.22 degré
+Coup 8: Frappe a gauche, la lance est à 89.44 degré
+Coup 9: Frappe a gauche, la lance est à 82.28 degré
+Coup 10: Frappe a droite, la lance est à 75.70 degré
+Coup 11: Frappe au centre, la lance est à 69.64 degré
+Coup 12: Frappe au centre, la lance est à 64.07 degré
+Coup 13: Frappe au centre, la lance est à 58.95 degré
+Coup 14: Frappe au centre, la lance est à 54.23 degré
+Rechauffe 3: de 49.89 à 99.89 degré</t>
+  </si>
+  <si>
+    <t>Coup 1: Frappe au centre, la lance est à 60.20 degré
+Coup 2: Frappe au centre, la lance est à 55.38 degré
+Coup 3: Frappe au centre, la lance est à 50.95 degré
+Rechauffe 1: de 46.88 à 96.88 degré
+Attends, la lance est à 96.88 degré
+Coup 4: Frappe a gauche, la lance est à 89.13 degré
+Coup 5: Frappe a gauche, la lance est à 82.00 degré
+Coup 6: Frappe a droite, la lance est à 75.44 degré
+Coup 7: Frappe au centre, la lance est à 69.40 degré
+Coup 8: Frappe au centre, la lance est à 63.85 degré
+Coup 9: Frappe au centre, la lance est à 58.74 degré
+Coup 10: Frappe au centre, la lance est à 54.04 degré
+Rechauffe 2: de 49.72 à 99.72 degré
+Attends, la lance est à 99.72 degré
+Attends, la lance est à 91.74 degré
+Coup 11: Frappe a gauche, la lance est à 84.40 degré
+Coup 12: Frappe a droite, la lance est à 77.65 degré
+Coup 13: Frappe a droite, la lance est à 71.44 degré
+Coup 14: Frappe au centre, la lance est à 65.72 degré
+Coup 15: Frappe au centre, la lance est à 60.47 degré
+Coup 16: Frappe au centre, la lance est à 55.63 degré
+Coup 17: Frappe au centre, la lance est à 51.18 degré
+Rechauffe 3: de 47.08 à 97.08 degré</t>
+  </si>
+  <si>
+    <t>Très bien, tu es pret a m'assister pour la forge de cette lance
+Je vais te dire la température initiale de la lance et tu devras me dire ce que je dois faire:
+Si la lance est strictement plus chaude que 90 degrés, Je dois attendre
+Si la lance est entre 90 degres compris et 80 degres non compris, Je dois frapper à droite
+Si la lance est entre 80 degres compris et 70 degres non compris, Je dois frapper à gauche
+Si la lance est entre 70 degres compris et 50 degres non compris, Je dois frapper au centre
+Si la lance est plus froide que 50 degres compris, je dois la réchauffer
+La lance sera prete lorsque soit, j'aurais frappé pour la 20eme fois, soit lorque je l'aurais réchauffée pour la 3eme fois
+Lorsque je rechauffe la lance, celle ci gagne 50 degres
+Lorsque j'attends ou que je la frappe, celle ci perd 8% de temperature
+Tu devras me dire precisement à quel temperature la lance est à chaque fois
+Et lorsque je la rechauffe, tu devras me dire sa temperature avant et après 
+L'input est un float N qui sera la temperature initiale de la lance
+Les outputs seront la suite d'informations que tu devras dire au forgeron. Les valeurs des températures auront toujours 2 décimales
+Regarde les exemples pour voir exactements ce qui est attendu</t>
+  </si>
+  <si>
+    <t>Pour afficher une valeur arrondie au 2 premeres decimale, tu peux utilser ceci
+{temp:.2f}</t>
+  </si>
+  <si>
+    <t>Coup 1: Frappe au centre, la lance est à 70.00 degré
+Coup 2: Frappe au centre, la lance est à 64.40 degré
+Coup 3: Frappe au centre, la lance est à 59.25 degré
+Coup 4: Frappe au centre, la lance est à 54.51 degré
+Coup 5: Frappe au centre, la lance est à 50.15 degré
+Rechauffe 1: de 46.14 à 96.14 degré
+Attends, la lance est à 96.14 degré
+Coup 6: Frappe a gauche, la lance est à 88.44 degré
+Coup 7: Frappe a gauche, la lance est à 81.37 degré
+Coup 8: Frappe a droite, la lance est à 74.86 degré
+Coup 9: Frappe au centre, la lance est à 68.87 degré
+Coup 10: Frappe au centre, la lance est à 63.36 degré
+Coup 11: Frappe au centre, la lance est à 58.29 degré
+Coup 12: Frappe au centre, la lance est à 53.63 degré
+Rechauffe 2: de 49.34 à 99.34 degré
+Attends, la lance est à 99.34 degré
+Attends, la lance est à 91.39 degré
+Coup 13: Frappe a gauche, la lance est à 84.08 degré
+Coup 14: Frappe a droite, la lance est à 77.35 degré
+Coup 15: Frappe a droite, la lance est à 71.17 degré
+Coup 16: Frappe au centre, la lance est à 65.47 degré
+Coup 17: Frappe au centre, la lance est à 60.23 degré
+Coup 18: Frappe au centre, la lance est à 55.42 degré
+Coup 19: Frappe au centre, la lance est à 50.98 degré
+Rechauffe 3: de 46.90 à 96.90 degré</t>
+  </si>
+  <si>
+    <t>Attends, la lance est à 95.71 degré
+Coup 1: Frappe a gauche, la lance est à 88.05 degré
+Coup 2: Frappe a gauche, la lance est à 81.01 degré
+Coup 3: Frappe a droite, la lance est à 74.53 degré
+Coup 4: Frappe au centre, la lance est à 68.57 degré
+Coup 5: Frappe au centre, la lance est à 63.08 degré
+Coup 6: Frappe au centre, la lance est à 58.03 degré
+Coup 7: Frappe au centre, la lance est à 53.39 degré
+Rechauffe 1: de 49.12 à 99.12 degré
+Attends, la lance est à 99.12 degré
+Attends, la lance est à 91.19 degré
+Coup 8: Frappe a gauche, la lance est à 83.90 degré
+Coup 9: Frappe a droite, la lance est à 77.18 degré
+Coup 10: Frappe a droite, la lance est à 71.01 degré
+Coup 11: Frappe au centre, la lance est à 65.33 degré
+Coup 12: Frappe au centre, la lance est à 60.10 degré
+Coup 13: Frappe au centre, la lance est à 55.29 degré
+Coup 14: Frappe au centre, la lance est à 50.87 degré
+Rechauffe 2: de 46.80 à 96.80 degré
+Attends, la lance est à 96.80 degré
+Coup 15: Frappe a gauche, la lance est à 89.06 degré
+Coup 16: Frappe a gauche, la lance est à 81.93 degré
+Coup 17: Frappe a droite, la lance est à 75.38 degré
+Coup 18: Frappe au centre, la lance est à 69.35 degré
+Coup 19: Frappe au centre, la lance est à 63.80 degré
+Coup 20: Frappe au centre, la lance est à 58.70 degré</t>
+  </si>
+  <si>
+    <t>95.71</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -502,6 +660,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF212529"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -524,7 +688,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -532,6 +696,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -868,8 +1033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95F0EE0D-D391-4AA7-AF3E-FA9E64764AC4}">
   <dimension ref="A1:Y11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H5" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" topLeftCell="G8" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1352,7 +1517,7 @@
       <c r="X7" s="1"/>
       <c r="Y7" s="1"/>
     </row>
-    <row r="8" spans="1:25" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25" ht="409.6" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>3</v>
       </c>
@@ -1365,27 +1530,29 @@
       <c r="D8" s="1">
         <v>1</v>
       </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>65</v>
+      <c r="E8" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F8" s="3">
+        <v>100</v>
+      </c>
+      <c r="G8" s="3">
+        <v>50</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>89</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>62</v>
+        <v>90</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>64</v>
+        <v>91</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>67</v>
+        <v>93</v>
       </c>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
@@ -1394,23 +1561,23 @@
       <c r="Q8" s="1">
         <v>3</v>
       </c>
-      <c r="R8" s="1" t="s">
-        <v>61</v>
+      <c r="R8" s="3">
+        <v>100</v>
       </c>
       <c r="S8" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="T8" s="1" t="s">
-        <v>63</v>
+        <v>90</v>
+      </c>
+      <c r="T8" s="1">
+        <v>70</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="V8" s="1" t="s">
-        <v>68</v>
+        <v>95</v>
+      </c>
+      <c r="V8" s="3" t="s">
+        <v>97</v>
       </c>
       <c r="W8" s="1" t="s">
-        <v>69</v>
+        <v>96</v>
       </c>
       <c r="X8" s="1"/>
       <c r="Y8" s="1"/>

</xml_diff>

<commit_message>
Correction bug diffictulté + taverne temporium + affichage score ecran de victoire
</commit_message>
<xml_diff>
--- a/Quete/Aventure.xlsx
+++ b/Quete/Aventure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\Python_Apprendre_Autrement\Quete\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51BAE790-1932-41AC-BB9B-88717A7FE457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9285D1AB-3EB5-4611-92B3-11E38C60F425}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0CA7E0B7-CDFC-4FD5-BEF9-F0FFA02D3C1D}"/>
   </bookViews>
@@ -1033,8 +1033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95F0EE0D-D391-4AA7-AF3E-FA9E64764AC4}">
   <dimension ref="A1:Y11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G8" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+    <sheetView tabSelected="1" topLeftCell="L5" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="Z5" sqref="Z5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1335,7 +1335,7 @@
         <v>3</v>
       </c>
       <c r="D5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1">
@@ -1379,7 +1379,7 @@
         <v>75</v>
       </c>
       <c r="V5" s="1">
-        <v>84</v>
+        <v>40</v>
       </c>
       <c r="W5" s="1" t="s">
         <v>76</v>
@@ -1402,7 +1402,7 @@
         <v>4</v>
       </c>
       <c r="D6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
@@ -1528,7 +1528,7 @@
         <v>6</v>
       </c>
       <c r="D8" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>94</v>

</xml_diff>